<commit_message>
Nguyen Trong Tien add link
</commit_message>
<xml_diff>
--- a/BaiNopKTLinkGitHub_Tiet_6_8.xlsx
+++ b/BaiNopKTLinkGitHub_Tiet_6_8.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Họ và tên</t>
   </si>
@@ -25,6 +25,9 @@
   </si>
   <si>
     <t>Link github</t>
+  </si>
+  <si>
+    <t>Nguyen Trong Tien</t>
   </si>
 </sst>
 </file>
@@ -72,6 +75,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -119,7 +125,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -154,7 +160,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -363,15 +369,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D2"/>
+  <dimension ref="A2:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
   </cols>
@@ -388,6 +394,14 @@
       </c>
       <c r="D2" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>6690007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>